<commit_message>
Namespace og identifikator vist
Namespace ikke skjult længere & begrebsidentifikator tilføjet
</commit_message>
<xml_diff>
--- a/concept-list-template/Begrebsliste_i_tabelformat_skabelon.xlsx
+++ b/concept-list-template/Begrebsliste_i_tabelformat_skabelon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="Denne_projektmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\KDA\Initiativ 8.1\4.1 Regler for begrebs- og datamodellering\- Ressource - FDA-udgivne værktøjer (v. 2.0)\Begrebslisteskabelon\v0.10.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B025870\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>prefLabel (da)</t>
   </si>
@@ -314,9 +314,6 @@
     <t>Namespace</t>
   </si>
   <si>
-    <t>Tilhørere emneområde</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modelansvarlig </t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>Tilhører emneområde</t>
+  </si>
+  <si>
+    <t>Identifikator</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -664,15 +664,127 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,7 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -739,12 +851,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2214,7 +2336,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>352424</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>17145</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2249,16 +2371,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2560,10 +2682,10 @@
   <sheetPr codeName="Ark1">
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A2:B15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,87 +2694,88 @@
     <col min="2" max="3" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="14"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="14"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
-        <v>47</v>
       </c>
       <c r="B15" s="5"/>
     </row>
@@ -2679,10 +2802,10 @@
     <tabColor rgb="FFC00000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2696,9 +2819,10 @@
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2724,7 +2848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>28</v>
       </c>
@@ -2750,10 +2874,13 @@
         <v>18</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="2"/>
       <c r="C3" s="6"/>
@@ -2765,8 +2892,11 @@
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2776,8 +2906,9 @@
       <c r="G4" s="9"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2787,8 +2918,9 @@
       <c r="G5" s="9"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2798,8 +2930,9 @@
       <c r="G6" s="9"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2809,8 +2942,9 @@
       <c r="G7" s="9"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2820,8 +2954,9 @@
       <c r="G8" s="9"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2831,8 +2966,9 @@
       <c r="G9" s="9"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2842,8 +2978,9 @@
       <c r="G10" s="9"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2853,8 +2990,9 @@
       <c r="G11" s="9"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2864,8 +3002,9 @@
       <c r="G12" s="9"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2875,8 +3014,9 @@
       <c r="G13" s="9"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2886,8 +3026,9 @@
       <c r="G14" s="9"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2897,8 +3038,9 @@
       <c r="G15" s="9"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2908,8 +3050,9 @@
       <c r="G16" s="9"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2919,8 +3062,9 @@
       <c r="G17" s="9"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2930,8 +3074,9 @@
       <c r="G18" s="9"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2941,8 +3086,9 @@
       <c r="G19" s="9"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2952,8 +3098,9 @@
       <c r="G20" s="9"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2963,8 +3110,9 @@
       <c r="G21" s="9"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2974,8 +3122,9 @@
       <c r="G22" s="9"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2985,8 +3134,9 @@
       <c r="G23" s="9"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2996,8 +3146,9 @@
       <c r="G24" s="9"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3007,8 +3158,9 @@
       <c r="G25" s="9"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3018,8 +3170,9 @@
       <c r="G26" s="9"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3029,8 +3182,9 @@
       <c r="G27" s="9"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3040,8 +3194,9 @@
       <c r="G28" s="9"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3051,12 +3206,14 @@
       <c r="G29" s="9"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1 I3:I1048576">
       <formula1>"Ja,Nej"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="J1:J1048576"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3069,10 +3226,10 @@
     <tabColor rgb="FFC00000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3085,17 +3242,19 @@
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="16" max="17" width="15.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="18" width="15.28515625" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="12" customFormat="1" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3121,25 +3280,28 @@
         <v>14</v>
       </c>
       <c r="J1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -3152,8 +3314,9 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:15" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:16" s="11" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>31</v>
       </c>
@@ -3179,763 +3342,810 @@
         <v>18</v>
       </c>
       <c r="I3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="M3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="N3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="O3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="27"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="26"/>
       <c r="M4" s="27"/>
       <c r="N4" s="27"/>
-      <c r="O4" s="28"/>
-    </row>
-    <row r="5" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O4" s="27"/>
+      <c r="P4" s="28"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="27"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="26"/>
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
-    </row>
-    <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O5" s="27"/>
+      <c r="P5" s="28"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="27"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="27"/>
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
-    </row>
-    <row r="7" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O6" s="27"/>
+      <c r="P6" s="28"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="27"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
-      <c r="O7" s="28"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O7" s="27"/>
+      <c r="P7" s="28"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="27"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
-      <c r="O8" s="28"/>
-    </row>
-    <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O8" s="27"/>
+      <c r="P8" s="28"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="27"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
-      <c r="O9" s="28"/>
-    </row>
-    <row r="10" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O9" s="27"/>
+      <c r="P9" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="27"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
-    </row>
-    <row r="11" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O10" s="27"/>
+      <c r="P10" s="28"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="27"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="37"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
-      <c r="O11" s="28"/>
-    </row>
-    <row r="12" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O11" s="27"/>
+      <c r="P11" s="28"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="27"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
-    </row>
-    <row r="13" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O12" s="27"/>
+      <c r="P12" s="28"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="27"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
-      <c r="O13" s="28"/>
-    </row>
-    <row r="14" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
       <c r="F14" s="27"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="27"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
-    </row>
-    <row r="15" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O14" s="27"/>
+      <c r="P14" s="28"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="27"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="37"/>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
       <c r="N15" s="27"/>
-      <c r="O15" s="28"/>
-    </row>
-    <row r="16" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O15" s="27"/>
+      <c r="P15" s="28"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="27"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="37"/>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
-    </row>
-    <row r="17" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O16" s="27"/>
+      <c r="P16" s="28"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="27"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="37"/>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
       <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
-    </row>
-    <row r="18" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O17" s="27"/>
+      <c r="P17" s="28"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="27"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="37"/>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
       <c r="N18" s="27"/>
-      <c r="O18" s="28"/>
-    </row>
-    <row r="19" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O18" s="27"/>
+      <c r="P18" s="28"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="27"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="37"/>
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
       <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
-    </row>
-    <row r="20" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O19" s="27"/>
+      <c r="P19" s="28"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="27"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="37"/>
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
       <c r="N20" s="27"/>
-      <c r="O20" s="28"/>
-    </row>
-    <row r="21" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O20" s="27"/>
+      <c r="P20" s="28"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="27"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="37"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
-      <c r="O21" s="28"/>
-    </row>
-    <row r="22" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O21" s="27"/>
+      <c r="P21" s="28"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="27"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="37"/>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
       <c r="N22" s="27"/>
-      <c r="O22" s="28"/>
-    </row>
-    <row r="23" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O22" s="27"/>
+      <c r="P22" s="28"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="27"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="37"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
-      <c r="O23" s="28"/>
-    </row>
-    <row r="24" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O23" s="27"/>
+      <c r="P23" s="28"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="27"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="37"/>
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
-    </row>
-    <row r="25" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O24" s="27"/>
+      <c r="P24" s="28"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="27"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="37"/>
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
-      <c r="O25" s="28"/>
-    </row>
-    <row r="26" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O25" s="27"/>
+      <c r="P25" s="28"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="29"/>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="27"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="37"/>
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
-      <c r="O26" s="28"/>
-    </row>
-    <row r="27" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O26" s="27"/>
+      <c r="P26" s="28"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="27"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="37"/>
       <c r="L27" s="27"/>
       <c r="M27" s="27"/>
       <c r="N27" s="27"/>
-      <c r="O27" s="28"/>
-    </row>
-    <row r="28" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O27" s="27"/>
+      <c r="P27" s="28"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="27"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="37"/>
       <c r="L28" s="27"/>
       <c r="M28" s="27"/>
       <c r="N28" s="27"/>
-      <c r="O28" s="28"/>
-    </row>
-    <row r="29" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O28" s="27"/>
+      <c r="P28" s="28"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="27"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="37"/>
       <c r="L29" s="27"/>
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
-      <c r="O29" s="28"/>
-    </row>
-    <row r="30" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O29" s="27"/>
+      <c r="P29" s="28"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="27"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="37"/>
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
-      <c r="O30" s="28"/>
-    </row>
-    <row r="31" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O30" s="27"/>
+      <c r="P30" s="28"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="27"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="37"/>
       <c r="L31" s="27"/>
       <c r="M31" s="27"/>
       <c r="N31" s="27"/>
-      <c r="O31" s="28"/>
-    </row>
-    <row r="32" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O31" s="27"/>
+      <c r="P31" s="28"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="29"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="27"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="37"/>
       <c r="L32" s="27"/>
       <c r="M32" s="27"/>
       <c r="N32" s="27"/>
-      <c r="O32" s="28"/>
-    </row>
-    <row r="33" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O32" s="27"/>
+      <c r="P32" s="28"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="29"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="27"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="37"/>
       <c r="L33" s="27"/>
       <c r="M33" s="27"/>
       <c r="N33" s="27"/>
-      <c r="O33" s="28"/>
-    </row>
-    <row r="34" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="O33" s="27"/>
+      <c r="P33" s="28"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="27"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="37"/>
       <c r="L34" s="27"/>
       <c r="M34" s="27"/>
       <c r="N34" s="27"/>
-      <c r="O34" s="28"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="27"/>
+      <c r="P34" s="28"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="29"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="27"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="37"/>
       <c r="L35" s="27"/>
       <c r="M35" s="27"/>
       <c r="N35" s="27"/>
-      <c r="O35" s="28"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="27"/>
+      <c r="P35" s="28"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="29"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="27"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="37"/>
       <c r="L36" s="27"/>
       <c r="M36" s="27"/>
       <c r="N36" s="27"/>
-      <c r="O36" s="28"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="27"/>
+      <c r="P36" s="28"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="29"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="27"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="37"/>
       <c r="L37" s="27"/>
       <c r="M37" s="27"/>
       <c r="N37" s="27"/>
-      <c r="O37" s="28"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="27"/>
+      <c r="P37" s="28"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="29"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="27"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="37"/>
       <c r="L38" s="27"/>
       <c r="M38" s="27"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="28"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="27"/>
+      <c r="P38" s="28"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="29"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="27"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="37"/>
       <c r="L39" s="27"/>
       <c r="M39" s="27"/>
       <c r="N39" s="27"/>
-      <c r="O39" s="28"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="27"/>
+      <c r="P39" s="28"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="29"/>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
       <c r="E40" s="27"/>
       <c r="F40" s="27"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="27"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="37"/>
       <c r="L40" s="27"/>
       <c r="M40" s="27"/>
       <c r="N40" s="27"/>
-      <c r="O40" s="28"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O40" s="27"/>
+      <c r="P40" s="28"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="27"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="37"/>
       <c r="L41" s="27"/>
       <c r="M41" s="27"/>
       <c r="N41" s="27"/>
-      <c r="O41" s="28"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O41" s="27"/>
+      <c r="P41" s="28"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="29"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="27"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="37"/>
       <c r="L42" s="27"/>
       <c r="M42" s="27"/>
       <c r="N42" s="27"/>
-      <c r="O42" s="28"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O42" s="27"/>
+      <c r="P42" s="28"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="27"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="37"/>
       <c r="L43" s="27"/>
       <c r="M43" s="27"/>
       <c r="N43" s="27"/>
-      <c r="O43" s="28"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O43" s="27"/>
+      <c r="P43" s="28"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="29"/>
       <c r="B44" s="26"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="27"/>
       <c r="F44" s="27"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="27"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="37"/>
       <c r="L44" s="27"/>
       <c r="M44" s="27"/>
       <c r="N44" s="27"/>
-      <c r="O44" s="28"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O44" s="27"/>
+      <c r="P44" s="28"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="29"/>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="27"/>
       <c r="F45" s="27"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="27"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="37"/>
       <c r="L45" s="27"/>
       <c r="M45" s="27"/>
       <c r="N45" s="27"/>
-      <c r="O45" s="28"/>
-    </row>
-    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O45" s="27"/>
+      <c r="P45" s="28"/>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46" s="31"/>
       <c r="C46" s="31"/>
       <c r="D46" s="31"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="32"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="38"/>
       <c r="L46" s="32"/>
       <c r="M46" s="32"/>
       <c r="N46" s="32"/>
-      <c r="O46" s="35"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="33"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I46">
       <formula1>"Ja,Nej"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="J1:J1048576"/>
   </dataValidations>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="68" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
fejlrettelse af datavalidering i metadatasektionen
</commit_message>
<xml_diff>
--- a/concept-list-template/Begrebsliste_i_tabelformat_skabelon.xlsx
+++ b/concept-list-template/Begrebsliste_i_tabelformat_skabelon.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7776"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Forretningsmetadata" sheetId="8" r:id="rId1"/>
@@ -2539,110 +2539,110 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="3" width="51.109375" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="3" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="15"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="15"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="15"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="15"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="15"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="15"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>40</v>
       </c>
@@ -2659,12 +2659,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>" core model (kernemodel),application model (anvendelsesmodel),"</formula1>
     </dataValidation>
-    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>" awaiting approval (afventer godkendelse),approved with remarks (godkendt med bemærkninger),approved (godkendt),not applicable (ikke relevant),"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
-      <formula1>" core model (kernemodel),application model (anvendelsesmodel),"</formula1>
-    </dataValidation>
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B9"/>
+    <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B7"/>
     <dataValidation showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B10"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2684,21 +2680,21 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="33.109375" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2724,7 +2720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -2759,7 +2755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -2774,7 +2770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2787,7 +2783,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -2800,7 +2796,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -2813,7 +2809,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2826,7 +2822,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2839,7 +2835,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -2852,7 +2848,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -2865,7 +2861,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -2878,7 +2874,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -2891,7 +2887,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -2904,7 +2900,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -2917,7 +2913,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2930,7 +2926,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -2943,7 +2939,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -2956,7 +2952,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -2969,7 +2965,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -2982,7 +2978,7 @@
       <c r="J19" s="8"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -2995,7 +2991,7 @@
       <c r="J20" s="8"/>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -3008,7 +3004,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="10"/>
     </row>
-    <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -3021,7 +3017,7 @@
       <c r="J22" s="8"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -3034,7 +3030,7 @@
       <c r="J23" s="8"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -3047,7 +3043,7 @@
       <c r="J24" s="8"/>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -3060,7 +3056,7 @@
       <c r="J25" s="8"/>
       <c r="K25" s="10"/>
     </row>
-    <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -3073,7 +3069,7 @@
       <c r="J26" s="8"/>
       <c r="K26" s="10"/>
     </row>
-    <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -3086,7 +3082,7 @@
       <c r="J27" s="8"/>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -3099,7 +3095,7 @@
       <c r="J28" s="8"/>
       <c r="K28" s="10"/>
     </row>
-    <row r="29" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -3133,29 +3129,29 @@
       <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
-    <col min="6" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="30.88671875" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.109375" customWidth="1"/>
-    <col min="15" max="15" width="18.88671875" customWidth="1"/>
-    <col min="16" max="16" width="26.109375" customWidth="1"/>
-    <col min="17" max="18" width="20.6640625" customWidth="1"/>
-    <col min="19" max="20" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="16" width="26.140625" customWidth="1"/>
+    <col min="17" max="18" width="20.7109375" customWidth="1"/>
+    <col min="19" max="20" width="15.28515625" customWidth="1"/>
     <col min="21" max="21" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3205,7 +3201,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3221,7 +3217,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>53</v>
       </c>
@@ -3277,7 +3273,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -3297,7 +3293,7 @@
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -3317,7 +3313,7 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -3337,7 +3333,7 @@
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -3357,7 +3353,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -3377,7 +3373,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -3397,7 +3393,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -3417,7 +3413,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -3437,7 +3433,7 @@
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -3457,7 +3453,7 @@
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -3477,7 +3473,7 @@
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -3497,7 +3493,7 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -3517,7 +3513,7 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -3537,7 +3533,7 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3557,7 +3553,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -3577,7 +3573,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -3597,7 +3593,7 @@
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -3617,7 +3613,7 @@
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -3637,7 +3633,7 @@
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -3657,7 +3653,7 @@
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -3677,7 +3673,7 @@
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -3697,7 +3693,7 @@
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -3717,7 +3713,7 @@
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -3737,7 +3733,7 @@
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -3757,7 +3753,7 @@
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -3777,7 +3773,7 @@
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -3797,7 +3793,7 @@
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -3817,7 +3813,7 @@
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -3837,7 +3833,7 @@
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3857,7 +3853,7 @@
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3877,7 +3873,7 @@
       <c r="Q33" s="7"/>
       <c r="R33" s="7"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3897,7 +3893,7 @@
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3917,7 +3913,7 @@
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3937,7 +3933,7 @@
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3957,7 +3953,7 @@
       <c r="Q37" s="7"/>
       <c r="R37" s="7"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3977,7 +3973,7 @@
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3997,7 +3993,7 @@
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -4017,7 +4013,7 @@
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -4037,7 +4033,7 @@
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -4057,7 +4053,7 @@
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -4077,7 +4073,7 @@
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -4097,7 +4093,7 @@
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -4117,7 +4113,7 @@
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -4159,24 +4155,24 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="35.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="42.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>56</v>
       </c>
@@ -4190,7 +4186,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>30</v>
       </c>
@@ -4204,7 +4200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>8</v>
       </c>
@@ -4218,7 +4214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>32</v>
       </c>
@@ -4232,7 +4228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>35</v>
       </c>
@@ -4246,7 +4242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>33</v>
       </c>
@@ -4260,7 +4256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>36</v>
       </c>
@@ -4274,7 +4270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
         <v>71</v>
       </c>
@@ -4288,7 +4284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
         <v>31</v>
       </c>
@@ -4302,7 +4298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
         <v>37</v>
       </c>
@@ -4316,7 +4312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
         <v>21</v>
       </c>
@@ -4330,7 +4326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
         <v>80</v>
       </c>
@@ -4344,7 +4340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>9</v>
       </c>
@@ -4358,7 +4354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
         <v>39</v>
       </c>
@@ -4370,7 +4366,7 @@
       </c>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
         <v>22</v>
       </c>
@@ -4384,7 +4380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>17</v>
       </c>
@@ -4398,7 +4394,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>40</v>
       </c>
@@ -4412,12 +4408,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>56</v>
       </c>
@@ -4431,7 +4427,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
         <v>92</v>
       </c>
@@ -4445,7 +4441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
         <v>26</v>
       </c>
@@ -4459,7 +4455,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B27" s="22" t="s">
         <v>25</v>
       </c>
@@ -4473,7 +4469,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
         <v>24</v>
       </c>
@@ -4487,7 +4483,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
         <v>23</v>
       </c>
@@ -4501,7 +4497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B30" s="22" t="s">
         <v>27</v>
       </c>
@@ -4515,7 +4511,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B31" s="22" t="s">
         <v>28</v>
       </c>
@@ -4529,7 +4525,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="22" t="s">
         <v>22</v>
       </c>
@@ -4543,7 +4539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="22" t="s">
         <v>17</v>
       </c>
@@ -4557,7 +4553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
       <c r="B34" s="22" t="s">
         <v>41</v>
       </c>
@@ -4584,13 +4580,13 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -4598,7 +4594,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4606,7 +4602,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -4614,7 +4610,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -4622,7 +4618,7 @@
         <v>44455</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>

</xml_diff>